<commit_message>
Fixed map and retirement 12.3.25
</commit_message>
<xml_diff>
--- a/data/state/raw_source/unemployment/Hires.xlsx
+++ b/data/state/raw_source/unemployment/Hires.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA8D63D7-ABF8-480A-9664-871ECC6CFBAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F2F2CA85-71A2-4609-8061-8B24F790BE53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{09BADE62-848B-4E48-916B-F510266BE4CA}"/>
   </bookViews>
@@ -215,9 +215,6 @@
     <t>Hiring Levels Change from: June 2025 - July 2025(p)</t>
   </si>
   <si>
-    <t>Hiring Rates -7/24/2025</t>
-  </si>
-  <si>
     <t>Hiring Rates -5/1/2025</t>
   </si>
   <si>
@@ -233,6 +230,9 @@
   </si>
   <si>
     <t>Hiring Rates -4/1/2025</t>
+  </si>
+  <si>
+    <t>Hiring Rates -7/1/2024</t>
   </si>
 </sst>
 </file>
@@ -723,7 +723,7 @@
   <dimension ref="A1:M53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -751,22 +751,22 @@
         <v>58</v>
       </c>
       <c r="H1" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">

</xml_diff>